<commit_message>
refactor: Update decomposition method to use multiplicative instead of additive
</commit_message>
<xml_diff>
--- a/data/actividad-05.xlsx
+++ b/data/actividad-05.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\777--Programacion repos\Una\r\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B80992B-E971-4F8B-8994-70BA6D6C07BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1898DA1F-7025-430D-A465-2312E3F94E81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6796A659-03C7-4986-94B7-1825171FFE05}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6796A659-03C7-4986-94B7-1825171FFE05}"/>
   </bookViews>
   <sheets>
     <sheet name="2" sheetId="1" r:id="rId1"/>
+    <sheet name="1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="9">
   <si>
     <t>Año</t>
   </si>
@@ -46,6 +47,12 @@
   </si>
   <si>
     <t>IV</t>
+  </si>
+  <si>
+    <t>Mes</t>
+  </si>
+  <si>
+    <t>IPC</t>
   </si>
 </sst>
 </file>
@@ -399,7 +406,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47E6C89C-6988-40C5-9BEA-4EAB17A5A4AC}">
   <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+    <sheetView topLeftCell="A46" workbookViewId="0">
       <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
@@ -1035,4 +1042,1042 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{416A2E07-7EA1-4885-9DDA-040420BBFF58}">
+  <dimension ref="A1:C93"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C68" sqref="C68"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1999</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>30.21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1999</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>30.321000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1999</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>30.349</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1999</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>30.43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1999</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>30.433</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1999</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>30.536000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1999</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>30.655999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1999</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>30.69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1999</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>30.978000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1999</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>31.300999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1999</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>31.305</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1999</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>31.541</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2000</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>31.78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2000</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>31.777000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2000</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>31.872</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>2000</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17">
+        <v>31.914000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>2000</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18">
+        <v>31.975999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2000</v>
+      </c>
+      <c r="B19">
+        <v>6</v>
+      </c>
+      <c r="C19">
+        <v>32.173000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>2000</v>
+      </c>
+      <c r="B20">
+        <v>7</v>
+      </c>
+      <c r="C20">
+        <v>32.33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>2000</v>
+      </c>
+      <c r="B21">
+        <v>8</v>
+      </c>
+      <c r="C21">
+        <v>32.481000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2000</v>
+      </c>
+      <c r="B22">
+        <v>9</v>
+      </c>
+      <c r="C22">
+        <v>32.561</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>2000</v>
+      </c>
+      <c r="B23">
+        <v>10</v>
+      </c>
+      <c r="C23">
+        <v>32.567999999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>2000</v>
+      </c>
+      <c r="B24">
+        <v>11</v>
+      </c>
+      <c r="C24">
+        <v>32.744</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2000</v>
+      </c>
+      <c r="B25">
+        <v>12</v>
+      </c>
+      <c r="C25">
+        <v>33.021000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>2001</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>33.348999999999997</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>2001</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27">
+        <v>33.487000000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>2001</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28">
+        <v>33.613999999999997</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>2001</v>
+      </c>
+      <c r="B29">
+        <v>4</v>
+      </c>
+      <c r="C29">
+        <v>33.786000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>2001</v>
+      </c>
+      <c r="B30">
+        <v>5</v>
+      </c>
+      <c r="C30">
+        <v>33.856000000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>2001</v>
+      </c>
+      <c r="B31">
+        <v>6</v>
+      </c>
+      <c r="C31">
+        <v>34.011000000000003</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>2001</v>
+      </c>
+      <c r="B32">
+        <v>7</v>
+      </c>
+      <c r="C32">
+        <v>33.984000000000002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>2001</v>
+      </c>
+      <c r="B33">
+        <v>8</v>
+      </c>
+      <c r="C33">
+        <v>34.293999999999997</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>2001</v>
+      </c>
+      <c r="B34">
+        <v>9</v>
+      </c>
+      <c r="C34">
+        <v>34.406999999999996</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>2001</v>
+      </c>
+      <c r="B35">
+        <v>10</v>
+      </c>
+      <c r="C35">
+        <v>34.441000000000003</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>2001</v>
+      </c>
+      <c r="B36">
+        <v>11</v>
+      </c>
+      <c r="C36">
+        <v>34.497999999999998</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>2001</v>
+      </c>
+      <c r="B37">
+        <v>12</v>
+      </c>
+      <c r="C37">
+        <v>34.659999999999997</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>2002</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <v>34.814</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>2002</v>
+      </c>
+      <c r="B39">
+        <v>2</v>
+      </c>
+      <c r="C39">
+        <v>34.923000000000002</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>2002</v>
+      </c>
+      <c r="B40">
+        <v>3</v>
+      </c>
+      <c r="C40">
+        <v>35.113</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>2002</v>
+      </c>
+      <c r="B41">
+        <v>4</v>
+      </c>
+      <c r="C41">
+        <v>35.335000000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>2002</v>
+      </c>
+      <c r="B42">
+        <v>5</v>
+      </c>
+      <c r="C42">
+        <v>35.402999999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>2002</v>
+      </c>
+      <c r="B43">
+        <v>6</v>
+      </c>
+      <c r="C43">
+        <v>35.665999999999997</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>2002</v>
+      </c>
+      <c r="B44">
+        <v>7</v>
+      </c>
+      <c r="C44">
+        <v>35.799999999999997</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>2002</v>
+      </c>
+      <c r="B45">
+        <v>8</v>
+      </c>
+      <c r="C45">
+        <v>36.036999999999999</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>2002</v>
+      </c>
+      <c r="B46">
+        <v>9</v>
+      </c>
+      <c r="C46">
+        <v>36.200000000000003</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>2002</v>
+      </c>
+      <c r="B47">
+        <v>10</v>
+      </c>
+      <c r="C47">
+        <v>36.225999999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>2002</v>
+      </c>
+      <c r="B48">
+        <v>11</v>
+      </c>
+      <c r="C48">
+        <v>36.462000000000003</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>2002</v>
+      </c>
+      <c r="B49">
+        <v>12</v>
+      </c>
+      <c r="C49">
+        <v>36.585999999999999</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>2003</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50">
+        <v>37.116999999999997</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>2003</v>
+      </c>
+      <c r="B51">
+        <v>2</v>
+      </c>
+      <c r="C51">
+        <v>37.424999999999997</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>2003</v>
+      </c>
+      <c r="B52">
+        <v>3</v>
+      </c>
+      <c r="C52">
+        <v>37.753999999999998</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>2003</v>
+      </c>
+      <c r="B53">
+        <v>4</v>
+      </c>
+      <c r="C53">
+        <v>38.351999999999997</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>2003</v>
+      </c>
+      <c r="B54">
+        <v>5</v>
+      </c>
+      <c r="C54">
+        <v>38.761000000000003</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>2003</v>
+      </c>
+      <c r="B55">
+        <v>6</v>
+      </c>
+      <c r="C55">
+        <v>39.076000000000001</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>2003</v>
+      </c>
+      <c r="B56">
+        <v>7</v>
+      </c>
+      <c r="C56">
+        <v>40.078000000000003</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>2003</v>
+      </c>
+      <c r="B57">
+        <v>8</v>
+      </c>
+      <c r="C57">
+        <v>40.722000000000001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>2003</v>
+      </c>
+      <c r="B58">
+        <v>9</v>
+      </c>
+      <c r="C58">
+        <v>41.691000000000003</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>2003</v>
+      </c>
+      <c r="B59">
+        <v>10</v>
+      </c>
+      <c r="C59">
+        <v>42.223999999999997</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>2003</v>
+      </c>
+      <c r="B60">
+        <v>11</v>
+      </c>
+      <c r="C60">
+        <v>42.744</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>2003</v>
+      </c>
+      <c r="B61">
+        <v>12</v>
+      </c>
+      <c r="C61">
+        <v>44.405000000000001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>2004</v>
+      </c>
+      <c r="B62">
+        <v>1</v>
+      </c>
+      <c r="C62">
+        <v>45.996000000000002</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>2004</v>
+      </c>
+      <c r="B63">
+        <v>2</v>
+      </c>
+      <c r="C63">
+        <v>47.033000000000001</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>2004</v>
+      </c>
+      <c r="B64">
+        <v>3</v>
+      </c>
+      <c r="C64">
+        <v>47.396000000000001</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>2004</v>
+      </c>
+      <c r="B65">
+        <v>4</v>
+      </c>
+      <c r="C65">
+        <v>48.040999999999997</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>2004</v>
+      </c>
+      <c r="B66">
+        <v>5</v>
+      </c>
+      <c r="C66">
+        <v>48.417000000000002</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>2004</v>
+      </c>
+      <c r="B67">
+        <v>6</v>
+      </c>
+      <c r="C67">
+        <v>48.896000000000001</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>2004</v>
+      </c>
+      <c r="B68">
+        <v>7</v>
+      </c>
+      <c r="C68">
+        <v>49.603000000000002</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>2004</v>
+      </c>
+      <c r="B69">
+        <v>8</v>
+      </c>
+      <c r="C69">
+        <v>50.128</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>2004</v>
+      </c>
+      <c r="B70">
+        <v>9</v>
+      </c>
+      <c r="C70">
+        <v>50.695999999999998</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>2004</v>
+      </c>
+      <c r="B71">
+        <v>10</v>
+      </c>
+      <c r="C71">
+        <v>51.701999999999998</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>2004</v>
+      </c>
+      <c r="B72">
+        <v>11</v>
+      </c>
+      <c r="C72">
+        <v>53.137</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>2004</v>
+      </c>
+      <c r="B73">
+        <v>12</v>
+      </c>
+      <c r="C73">
+        <v>53.552</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>2005</v>
+      </c>
+      <c r="B74">
+        <v>1</v>
+      </c>
+      <c r="C74">
+        <v>54.237000000000002</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>2005</v>
+      </c>
+      <c r="B75">
+        <v>2</v>
+      </c>
+      <c r="C75">
+        <v>54.536999999999999</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>2005</v>
+      </c>
+      <c r="B76">
+        <v>3</v>
+      </c>
+      <c r="C76">
+        <v>54.88</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>2005</v>
+      </c>
+      <c r="B77">
+        <v>4</v>
+      </c>
+      <c r="C77">
+        <v>55.344000000000001</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>2005</v>
+      </c>
+      <c r="B78">
+        <v>5</v>
+      </c>
+      <c r="C78">
+        <v>56.084000000000003</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>2005</v>
+      </c>
+      <c r="B79">
+        <v>6</v>
+      </c>
+      <c r="C79">
+        <v>57.036000000000001</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>2005</v>
+      </c>
+      <c r="B80">
+        <v>7</v>
+      </c>
+      <c r="C80">
+        <v>57.494</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>2005</v>
+      </c>
+      <c r="B81">
+        <v>8</v>
+      </c>
+      <c r="C81">
+        <v>57.991999999999997</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>2005</v>
+      </c>
+      <c r="B82">
+        <v>9</v>
+      </c>
+      <c r="C82">
+        <v>58.412999999999997</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>2005</v>
+      </c>
+      <c r="B83">
+        <v>10</v>
+      </c>
+      <c r="C83">
+        <v>58.713000000000001</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>2005</v>
+      </c>
+      <c r="B84">
+        <v>11</v>
+      </c>
+      <c r="C84">
+        <v>59.124000000000002</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>2005</v>
+      </c>
+      <c r="B85">
+        <v>12</v>
+      </c>
+      <c r="C85">
+        <v>59.606000000000002</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>2006</v>
+      </c>
+      <c r="B86">
+        <v>1</v>
+      </c>
+      <c r="C86">
+        <v>60.759</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>2006</v>
+      </c>
+      <c r="B87">
+        <v>2</v>
+      </c>
+      <c r="C87">
+        <v>61.893999999999998</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>2006</v>
+      </c>
+      <c r="B88">
+        <v>3</v>
+      </c>
+      <c r="C88">
+        <v>62.502000000000002</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>2006</v>
+      </c>
+      <c r="B89">
+        <v>4</v>
+      </c>
+      <c r="C89">
+        <v>62.939</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>2006</v>
+      </c>
+      <c r="B90">
+        <v>5</v>
+      </c>
+      <c r="C90">
+        <v>63.38</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>2006</v>
+      </c>
+      <c r="B91">
+        <v>6</v>
+      </c>
+      <c r="C91">
+        <v>63.633000000000003</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>2006</v>
+      </c>
+      <c r="B92">
+        <v>7</v>
+      </c>
+      <c r="C92">
+        <v>64.17</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>2006</v>
+      </c>
+      <c r="B93">
+        <v>8</v>
+      </c>
+      <c r="C93">
+        <v>64.787000000000006</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>